<commit_message>
completed student information form
</commit_message>
<xml_diff>
--- a/teacher.xlsx
+++ b/teacher.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java_netbean\StudentManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaProject\StudentManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D09548F-844A-4D24-93F3-F7E6FB9ACC0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0C4FD-1956-4157-94E0-8DFCFCA9FD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D93DEF0E-9E5E-4CFD-83AA-8A37395EBFAD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>thesi@gmail.com</t>
   </si>
@@ -130,6 +130,36 @@
   </si>
   <si>
     <t>Trần Mỹ Hạnh</t>
+  </si>
+  <si>
+    <t>Rank 1</t>
+  </si>
+  <si>
+    <t>No problem</t>
+  </si>
+  <si>
+    <t>Rank 7</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Rank 5</t>
+  </si>
+  <si>
+    <t>Reprimand</t>
+  </si>
+  <si>
+    <t>Rank 10</t>
+  </si>
+  <si>
+    <t>Rank 3</t>
+  </si>
+  <si>
+    <t>Rank 12</t>
+  </si>
+  <si>
+    <t>Rank 17</t>
   </si>
 </sst>
 </file>
@@ -641,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031DF760-193C-4C61-8773-5A05981EB4A4}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,9 +688,10 @@
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="10" width="25.42578125" style="16" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="16" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1">
       <c r="A1" s="1">
         <v>202170021</v>
       </c>
@@ -694,8 +725,17 @@
       <c r="K1" s="16">
         <v>10000000</v>
       </c>
+      <c r="L1">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickBot="1">
+    <row r="2" spans="1:14" ht="16.5" thickBot="1">
       <c r="A2" s="9">
         <v>202170022</v>
       </c>
@@ -729,8 +769,17 @@
       <c r="K2" s="16">
         <v>10000000</v>
       </c>
+      <c r="L2">
+        <v>180</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:14" ht="26.25" customHeight="1" thickBot="1">
       <c r="A3" s="11">
         <v>202170023</v>
       </c>
@@ -764,8 +813,17 @@
       <c r="K3" s="16">
         <v>10000000</v>
       </c>
+      <c r="L3">
+        <v>150</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5" thickBot="1">
+    <row r="4" spans="1:14" ht="16.5" thickBot="1">
       <c r="A4" s="9">
         <v>202170024</v>
       </c>
@@ -799,8 +857,17 @@
       <c r="K4" s="16">
         <v>10000000</v>
       </c>
+      <c r="L4">
+        <v>120</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1">
+    <row r="5" spans="1:14" ht="16.5" thickBot="1">
       <c r="A5" s="11">
         <v>202170025</v>
       </c>
@@ -834,8 +901,17 @@
       <c r="K5" s="16">
         <v>10000000</v>
       </c>
+      <c r="L5">
+        <v>200</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="21.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:14" ht="21.75" customHeight="1" thickBot="1">
       <c r="A6" s="9">
         <v>202170026</v>
       </c>
@@ -869,8 +945,17 @@
       <c r="K6" s="16">
         <v>10000000</v>
       </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" thickBot="1">
+    <row r="7" spans="1:14" ht="16.5" thickBot="1">
       <c r="A7" s="11">
         <v>202170027</v>
       </c>
@@ -904,8 +989,17 @@
       <c r="K7" s="16">
         <v>10000000</v>
       </c>
+      <c r="L7">
+        <v>180</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:14" ht="27" thickBot="1">
       <c r="A8" s="9">
         <v>202170028</v>
       </c>
@@ -939,8 +1033,17 @@
       <c r="K8" s="16">
         <v>10000000</v>
       </c>
+      <c r="L8">
+        <v>160</v>
+      </c>
+      <c r="M8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" thickBot="1">
+    <row r="9" spans="1:14" ht="16.5" thickBot="1">
       <c r="A9" s="9">
         <v>20217009</v>
       </c>
@@ -974,8 +1077,17 @@
       <c r="K9" s="16">
         <v>10000000</v>
       </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickBot="1">
+    <row r="10" spans="1:14" ht="16.5" thickBot="1">
       <c r="A10" s="9">
         <v>202170010</v>
       </c>
@@ -1008,6 +1120,15 @@
       </c>
       <c r="K10" s="16">
         <v>10000000</v>
+      </c>
+      <c r="L10">
+        <v>170</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix database and excel file
</commit_message>
<xml_diff>
--- a/teacher.xlsx
+++ b/teacher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaProject\StudentManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E561DBEF-0781-4716-929E-4812F328BA5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52FE839-6171-43A4-9A73-EB018242CAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D93DEF0E-9E5E-4CFD-83AA-8A37395EBFAD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>thesi@gmail.com</t>
   </si>
@@ -130,6 +130,36 @@
   </si>
   <si>
     <t>Trần Mỹ Hạnh</t>
+  </si>
+  <si>
+    <t>Rank 1</t>
+  </si>
+  <si>
+    <t>No problem</t>
+  </si>
+  <si>
+    <t>Rank 7</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Rank 5</t>
+  </si>
+  <si>
+    <t>Reprimand</t>
+  </si>
+  <si>
+    <t>Rank 10</t>
+  </si>
+  <si>
+    <t>Rank 3</t>
+  </si>
+  <si>
+    <t>Rank 12</t>
+  </si>
+  <si>
+    <t>Rank 17</t>
   </si>
 </sst>
 </file>
@@ -641,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031DF760-193C-4C61-8773-5A05981EB4A4}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="L1" sqref="L1:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,9 +688,11 @@
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="10" width="25.42578125" style="16" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="16" customWidth="1"/>
+    <col min="12" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1">
       <c r="A1" s="1">
         <v>202170021</v>
       </c>
@@ -694,8 +726,17 @@
       <c r="K1" s="16">
         <v>10000000</v>
       </c>
+      <c r="L1">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickBot="1">
+    <row r="2" spans="1:14" ht="16.5" thickBot="1">
       <c r="A2" s="9">
         <v>202170022</v>
       </c>
@@ -729,8 +770,17 @@
       <c r="K2" s="16">
         <v>10000000</v>
       </c>
+      <c r="L2">
+        <v>180</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:14" ht="26.25" customHeight="1" thickBot="1">
       <c r="A3" s="11">
         <v>202170023</v>
       </c>
@@ -764,8 +814,17 @@
       <c r="K3" s="16">
         <v>10000000</v>
       </c>
+      <c r="L3">
+        <v>150</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5" thickBot="1">
+    <row r="4" spans="1:14" ht="16.5" thickBot="1">
       <c r="A4" s="9">
         <v>202170024</v>
       </c>
@@ -799,8 +858,17 @@
       <c r="K4" s="16">
         <v>10000000</v>
       </c>
+      <c r="L4">
+        <v>120</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1">
+    <row r="5" spans="1:14" ht="16.5" thickBot="1">
       <c r="A5" s="11">
         <v>202170025</v>
       </c>
@@ -834,8 +902,17 @@
       <c r="K5" s="16">
         <v>10000000</v>
       </c>
+      <c r="L5">
+        <v>200</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="21.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:14" ht="21.75" customHeight="1" thickBot="1">
       <c r="A6" s="9">
         <v>202170026</v>
       </c>
@@ -869,8 +946,17 @@
       <c r="K6" s="16">
         <v>10000000</v>
       </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" thickBot="1">
+    <row r="7" spans="1:14" ht="16.5" thickBot="1">
       <c r="A7" s="11">
         <v>202170027</v>
       </c>
@@ -904,8 +990,17 @@
       <c r="K7" s="16">
         <v>10000000</v>
       </c>
+      <c r="L7">
+        <v>180</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:14" ht="27" thickBot="1">
       <c r="A8" s="9">
         <v>202170028</v>
       </c>
@@ -939,8 +1034,17 @@
       <c r="K8" s="16">
         <v>10000000</v>
       </c>
+      <c r="L8">
+        <v>160</v>
+      </c>
+      <c r="M8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" thickBot="1">
+    <row r="9" spans="1:14" ht="16.5" thickBot="1">
       <c r="A9" s="9">
         <v>20217009</v>
       </c>
@@ -974,8 +1078,17 @@
       <c r="K9" s="16">
         <v>10000000</v>
       </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickBot="1">
+    <row r="10" spans="1:14" ht="16.5" thickBot="1">
       <c r="A10" s="9">
         <v>202170010</v>
       </c>
@@ -1008,6 +1121,15 @@
       </c>
       <c r="K10" s="16">
         <v>10000000</v>
+      </c>
+      <c r="L10">
+        <v>170</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>